<commit_message>
Cadastro Novo, Atualiza e Exclui FINISHED
</commit_message>
<xml_diff>
--- a/Tabela_Aluno_Campos.xlsx
+++ b/Tabela_Aluno_Campos.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jribe\eclipse-workspace\MariaLobatoGenteJovem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F617B2C-4869-4FD3-B8A5-6016B76F3FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D764F363-A832-401C-9ED7-5169B657E3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BCEF3EA5-B1A7-48E7-889E-E8D820FE6D87}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="1" xr2:uid="{BCEF3EA5-B1A7-48E7-889E-E8D820FE6D87}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="OLE_LINK1" localSheetId="0">Planilha1!#REF!</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="79">
   <si>
     <t>Integer</t>
   </si>
@@ -254,9 +255,6 @@
     <t>NumeroNIS</t>
   </si>
   <si>
-    <t>EncaminhaOutra)</t>
-  </si>
-  <si>
     <t>InserT DB</t>
   </si>
   <si>
@@ -270,13 +268,22 @@
   </si>
   <si>
     <t>int(02)</t>
+  </si>
+  <si>
+    <t>findByCPF</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>INICIALIZA_FORMULARIO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +311,53 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFBDC1C6"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF717171"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -325,7 +379,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -361,11 +415,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -393,6 +458,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -708,27 +796,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B5FD43-F609-42B4-90F4-71811082D573}">
-  <dimension ref="A1:J104"/>
+  <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J52" sqref="J3:J52"/>
+    <sheetView topLeftCell="C45" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="46.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="30" style="9" customWidth="1"/>
-    <col min="8" max="8" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18" style="9" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="43.28515625" customWidth="1"/>
-    <col min="10" max="10" width="45" customWidth="1"/>
+    <col min="10" max="10" width="42.140625" customWidth="1"/>
+    <col min="11" max="11" width="33.5703125" style="10" customWidth="1"/>
+    <col min="12" max="12" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>59</v>
       </c>
@@ -750,13 +840,19 @@
       <c r="G1" s="9"/>
       <c r="H1" s="7"/>
       <c r="I1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -773,7 +869,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="2" t="str">
-        <f>_xlfn.CONCAT(B2," ",C2," ",D2," ,")</f>
+        <f t="shared" ref="F2:F33" si="0">_xlfn.CONCAT(B2," ",C2," ",D2," ,")</f>
         <v>id int(11)  NOT NULL  AUTO_INCREMENT ,</v>
       </c>
       <c r="G2" s="9">
@@ -790,8 +886,16 @@
         <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H2,",",G2,");")</f>
         <v>Constraints.setTextFieldMaxLength(idid,11);</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="10" t="str">
+        <f>_xlfn.CONCAT("obj.set",H2,"(rs.getString(",$K$54,H2,$K$54,"));")</f>
+        <v>obj.setid(rs.getString("id"));</v>
+      </c>
+      <c r="L2" t="str">
+        <f>_xlfn.CONCAT("id",H2,".setText(aluno.get",H2,"());")</f>
+        <v>idid.setText(aluno.getid());</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -823,11 +927,19 @@
         <v>st.setString(2,obj.getNomeAluno());</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J52" si="0">_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H3,",",G3,");")</f>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H3,",",G3,");")</f>
         <v>Constraints.setTextFieldMaxLength(idNomeAluno,60);</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="10" t="str">
+        <f>_xlfn.CONCAT("obj.set",H3,"(rs.getString(",$K$54,H3,$K$54,"));")</f>
+        <v>obj.setNomeAluno(rs.getString("NomeAluno"));</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L52" si="1">_xlfn.CONCAT("id",H3,".setText(aluno.get",H3,"());")</f>
+        <v>idNomeAluno.setText(aluno.getNomeAluno());</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -848,22 +960,30 @@
         <v>DataCadastro varchar(10) NOT NULL ,</v>
       </c>
       <c r="G4" s="9" t="str">
-        <f t="shared" ref="G4:G52" si="1">MID(C4,9,2)</f>
+        <f>MID(C4,9,2)</f>
         <v>10</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" ref="I4:I52" si="2">_xlfn.CONCAT("st.setString(",E4,",obj.get",H4,"());")</f>
+        <f>_xlfn.CONCAT("st.setString(",E4,",obj.get",H4,"());")</f>
         <v>st.setString(3,obj.getDataCadastro());</v>
       </c>
       <c r="J4" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H4,",",G4,");")</f>
         <v>Constraints.setTextFieldMaxLength(idDataCadastro,10);</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K4" s="10" t="str">
+        <f t="shared" ref="K4:K16" si="2">_xlfn.CONCAT("obj.set",H4,"(rs.getString(",$K$54,H4,$K$54,"));")</f>
+        <v>obj.setDataCadastro(rs.getString("DataCadastro"));</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="1"/>
+        <v>idDataCadastro.setText(aluno.getDataCadastro());</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -884,22 +1004,30 @@
         <v>Situacao varchar(10) NOT NULL ,</v>
       </c>
       <c r="G5" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C5,9,2)</f>
         <v>10</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="I5" t="str">
+        <f>_xlfn.CONCAT("st.setString(",E5,",obj.get",H5,"());")</f>
+        <v>st.setString(4,obj.getSituacao());</v>
+      </c>
+      <c r="J5" t="str">
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H5,",",G5,");")</f>
+        <v>Constraints.setTextFieldMaxLength(idSituacao,10);</v>
+      </c>
+      <c r="K5" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>st.setString(4,obj.getSituacao());</v>
-      </c>
-      <c r="J5" t="str">
-        <f t="shared" si="0"/>
-        <v>Constraints.setTextFieldMaxLength(idSituacao,10);</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>obj.setSituacao(rs.getString("Situacao"));</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="1"/>
+        <v>idSituacao.setText(aluno.getSituacao());</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -920,22 +1048,30 @@
         <v>RgAluno varchar(15) NOT NULL ,</v>
       </c>
       <c r="G6" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C6,9,2)</f>
         <v>15</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="I6" t="str">
+        <f>_xlfn.CONCAT("st.setString(",E6,",obj.get",H6,"());")</f>
+        <v>st.setString(5,obj.getRgAluno());</v>
+      </c>
+      <c r="J6" t="str">
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H6,",",G6,");")</f>
+        <v>Constraints.setTextFieldMaxLength(idRgAluno,15);</v>
+      </c>
+      <c r="K6" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>st.setString(5,obj.getRgAluno());</v>
-      </c>
-      <c r="J6" t="str">
-        <f t="shared" si="0"/>
-        <v>Constraints.setTextFieldMaxLength(idRgAluno,15);</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>obj.setRgAluno(rs.getString("RgAluno"));</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="1"/>
+        <v>idRgAluno.setText(aluno.getRgAluno());</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -956,22 +1092,30 @@
         <v>CpfAluno varchar(15)   ,</v>
       </c>
       <c r="G7" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C7,9,2)</f>
         <v>15</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I7" t="str">
+        <f>_xlfn.CONCAT("st.setString(",E7,",obj.get",H7,"());")</f>
+        <v>st.setString(6,obj.getCpfAluno());</v>
+      </c>
+      <c r="J7" t="str">
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H7,",",G7,");")</f>
+        <v>Constraints.setTextFieldMaxLength(idCpfAluno,15);</v>
+      </c>
+      <c r="K7" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>st.setString(6,obj.getCpfAluno());</v>
-      </c>
-      <c r="J7" t="str">
-        <f t="shared" si="0"/>
-        <v>Constraints.setTextFieldMaxLength(idCpfAluno,15);</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>obj.setCpfAluno(rs.getString("CpfAluno"));</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="1"/>
+        <v>idCpfAluno.setText(aluno.getCpfAluno());</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -992,22 +1136,30 @@
         <v>DataNascimentoAluno varchar(10) NOT NULL ,</v>
       </c>
       <c r="G8" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C8,9,2)</f>
         <v>10</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="I8" t="str">
+        <f>_xlfn.CONCAT("st.setString(",E8,",obj.get",H8,"());")</f>
+        <v>st.setString(7,obj.getDataNascimentoAluno());</v>
+      </c>
+      <c r="J8" t="str">
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H8,",",G8,");")</f>
+        <v>Constraints.setTextFieldMaxLength(idDataNascimentoAluno,10);</v>
+      </c>
+      <c r="K8" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>st.setString(7,obj.getDataNascimentoAluno());</v>
-      </c>
-      <c r="J8" t="str">
-        <f t="shared" si="0"/>
-        <v>Constraints.setTextFieldMaxLength(idDataNascimentoAluno,10);</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>obj.setDataNascimentoAluno(rs.getString("DataNascimentoAluno"));</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="1"/>
+        <v>idDataNascimentoAluno.setText(aluno.getDataNascimentoAluno());</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1028,22 +1180,30 @@
         <v>Sexo varchar(13) NOT NULL ,</v>
       </c>
       <c r="G9" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C9,9,2)</f>
         <v>13</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="I9" t="str">
+        <f>_xlfn.CONCAT("st.setString(",E9,",obj.get",H9,"());")</f>
+        <v>st.setString(8,obj.getSexo());</v>
+      </c>
+      <c r="J9" t="str">
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H9,",",G9,");")</f>
+        <v>Constraints.setTextFieldMaxLength(idSexo,13);</v>
+      </c>
+      <c r="K9" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>st.setString(8,obj.getSexo());</v>
-      </c>
-      <c r="J9" t="str">
-        <f t="shared" si="0"/>
-        <v>Constraints.setTextFieldMaxLength(idSexo,13);</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>obj.setSexo(rs.getString("Sexo"));</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="1"/>
+        <v>idSexo.setText(aluno.getSexo());</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1064,22 +1224,30 @@
         <v>NomeRuaAluno varchar(100) NOT NULL ,</v>
       </c>
       <c r="G10" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C10,9,2)</f>
         <v>10</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="I10" t="str">
+        <f>_xlfn.CONCAT("st.setString(",E10,",obj.get",H10,"());")</f>
+        <v>st.setString(9,obj.getNomeRuaAluno());</v>
+      </c>
+      <c r="J10" t="str">
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H10,",",G10,");")</f>
+        <v>Constraints.setTextFieldMaxLength(idNomeRuaAluno,10);</v>
+      </c>
+      <c r="K10" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>st.setString(9,obj.getNomeRuaAluno());</v>
-      </c>
-      <c r="J10" t="str">
-        <f t="shared" si="0"/>
-        <v>Constraints.setTextFieldMaxLength(idNomeRuaAluno,10);</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>obj.setNomeRuaAluno(rs.getString("NomeRuaAluno"));</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="1"/>
+        <v>idNomeRuaAluno.setText(aluno.getNomeRuaAluno());</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1087,7 +1255,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D11" t="s">
         <v>53</v>
@@ -1106,15 +1274,23 @@
         <v>11</v>
       </c>
       <c r="I11" t="str">
+        <f>_xlfn.CONCAT("st.setString(",E11,",obj.get",H11,"());")</f>
+        <v>st.setString(10,obj.getNumeroRuaAluno());</v>
+      </c>
+      <c r="J11" t="str">
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H11,",",G11,");")</f>
+        <v>Constraints.setTextFieldMaxLength(idNumeroRuaAluno,4);</v>
+      </c>
+      <c r="K11" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>st.setString(10,obj.getNumeroRuaAluno());</v>
-      </c>
-      <c r="J11" t="str">
-        <f t="shared" si="0"/>
-        <v>Constraints.setTextFieldMaxLength(idNumeroRuaAluno,4);</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>obj.setNumeroRuaAluno(rs.getString("NumeroRuaAluno"));</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="1"/>
+        <v>idNumeroRuaAluno.setText(aluno.getNumeroRuaAluno());</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1135,22 +1311,30 @@
         <v>BairroAluno varchar(60) NOT NULL ,</v>
       </c>
       <c r="G12" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C12,9,2)</f>
         <v>60</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I12" t="str">
+        <f>_xlfn.CONCAT("st.setString(",E12,",obj.get",H12,"());")</f>
+        <v>st.setString(11,obj.getBairroAluno());</v>
+      </c>
+      <c r="J12" t="str">
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H12,",",G12,");")</f>
+        <v>Constraints.setTextFieldMaxLength(idBairroAluno,60);</v>
+      </c>
+      <c r="K12" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>st.setString(11,obj.getBairroAluno());</v>
-      </c>
-      <c r="J12" t="str">
-        <f t="shared" si="0"/>
-        <v>Constraints.setTextFieldMaxLength(idBairroAluno,60);</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>obj.setBairroAluno(rs.getString("BairroAluno"));</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="1"/>
+        <v>idBairroAluno.setText(aluno.getBairroAluno());</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1171,22 +1355,30 @@
         <v>CepAluno varchar(20) NOT NULL ,</v>
       </c>
       <c r="G13" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C13,9,2)</f>
         <v>20</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I13" t="str">
+        <f>_xlfn.CONCAT("st.setString(",E13,",obj.get",H13,"());")</f>
+        <v>st.setString(12,obj.getCepAluno());</v>
+      </c>
+      <c r="J13" t="str">
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H13,",",G13,");")</f>
+        <v>Constraints.setTextFieldMaxLength(idCepAluno,20);</v>
+      </c>
+      <c r="K13" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>st.setString(12,obj.getCepAluno());</v>
-      </c>
-      <c r="J13" t="str">
-        <f t="shared" si="0"/>
-        <v>Constraints.setTextFieldMaxLength(idCepAluno,20);</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>obj.setCepAluno(rs.getString("CepAluno"));</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="1"/>
+        <v>idCepAluno.setText(aluno.getCepAluno());</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1207,22 +1399,30 @@
         <v>CelularAluno varchar(15)   ,</v>
       </c>
       <c r="G14" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C14,9,2)</f>
         <v>15</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I14" t="str">
+        <f>_xlfn.CONCAT("st.setString(",E14,",obj.get",H14,"());")</f>
+        <v>st.setString(13,obj.getCelularAluno());</v>
+      </c>
+      <c r="J14" t="str">
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H14,",",G14,");")</f>
+        <v>Constraints.setTextFieldMaxLength(idCelularAluno,15);</v>
+      </c>
+      <c r="K14" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>st.setString(13,obj.getCelularAluno());</v>
-      </c>
-      <c r="J14" t="str">
-        <f t="shared" si="0"/>
-        <v>Constraints.setTextFieldMaxLength(idCelularAluno,15);</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>obj.setCelularAluno(rs.getString("CelularAluno"));</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="1"/>
+        <v>idCelularAluno.setText(aluno.getCelularAluno());</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1243,22 +1443,30 @@
         <v>TelFixoAluno varchar(20)   ,</v>
       </c>
       <c r="G15" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C15,9,2)</f>
         <v>20</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I15" t="str">
+        <f>_xlfn.CONCAT("st.setString(",E15,",obj.get",H15,"());")</f>
+        <v>st.setString(14,obj.getTelFixoAluno());</v>
+      </c>
+      <c r="J15" t="str">
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H15,",",G15,");")</f>
+        <v>Constraints.setTextFieldMaxLength(idTelFixoAluno,20);</v>
+      </c>
+      <c r="K15" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>st.setString(14,obj.getTelFixoAluno());</v>
-      </c>
-      <c r="J15" t="str">
-        <f t="shared" si="0"/>
-        <v>Constraints.setTextFieldMaxLength(idTelFixoAluno,20);</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>obj.setTelFixoAluno(rs.getString("TelFixoAluno"));</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="1"/>
+        <v>idTelFixoAluno.setText(aluno.getTelFixoAluno());</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1279,22 +1487,30 @@
         <v>EmailAluno varchar(60)   ,</v>
       </c>
       <c r="G16" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C16,9,2)</f>
         <v>60</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="I16" t="str">
+        <f>_xlfn.CONCAT("st.setString(",E16,",obj.get",H16,"());")</f>
+        <v>st.setString(15,obj.getEmailAluno());</v>
+      </c>
+      <c r="J16" t="str">
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H16,",",G16,");")</f>
+        <v>Constraints.setTextFieldMaxLength(idEmailAluno,60);</v>
+      </c>
+      <c r="K16" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>st.setString(15,obj.getEmailAluno());</v>
-      </c>
-      <c r="J16" t="str">
-        <f t="shared" si="0"/>
-        <v>Constraints.setTextFieldMaxLength(idEmailAluno,60);</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>obj.setEmailAluno(rs.getString("EmailAluno"));</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="1"/>
+        <v>idEmailAluno.setText(aluno.getEmailAluno());</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1315,22 +1531,30 @@
         <v>EscolaAluno varchar(60) NOT NULL ,</v>
       </c>
       <c r="G17" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C17,9,2)</f>
         <v>60</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I17" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E17,",obj.get",H17,"());")</f>
         <v>st.setString(16,obj.getEscolaAluno());</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H17,",",G17,");")</f>
         <v>Constraints.setTextFieldMaxLength(idEscolaAluno,60);</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K17" s="10" t="str">
+        <f>_xlfn.CONCAT("obj.set",H17,"(rs.getString(",$K$54,H17,$K$54,"));")</f>
+        <v>obj.setEscolaAluno(rs.getString("EscolaAluno"));</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="1"/>
+        <v>idEscolaAluno.setText(aluno.getEscolaAluno());</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1351,22 +1575,30 @@
         <v>PeriodoAluno varchar(10) NOT NULL ,</v>
       </c>
       <c r="G18" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C18,9,2)</f>
         <v>10</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>18</v>
       </c>
       <c r="I18" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E18,",obj.get",H18,"());")</f>
         <v>st.setString(17,obj.getPeriodoAluno());</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H18,",",G18,");")</f>
         <v>Constraints.setTextFieldMaxLength(idPeriodoAluno,10);</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K18" s="10" t="str">
+        <f>_xlfn.CONCAT("obj.set",H18,"(rs.getString(",$K$54,H18,$K$54,"));")</f>
+        <v>obj.setPeriodoAluno(rs.getString("PeriodoAluno"));</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="1"/>
+        <v>idPeriodoAluno.setText(aluno.getPeriodoAluno());</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1387,22 +1619,30 @@
         <v>AnoEscolarAluno varchar(10) NOT NULL ,</v>
       </c>
       <c r="G19" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C19,9,2)</f>
         <v>10</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>19</v>
       </c>
       <c r="I19" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E19,",obj.get",H19,"());")</f>
         <v>st.setString(18,obj.getAnoEscolarAluno());</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H19,",",G19,");")</f>
         <v>Constraints.setTextFieldMaxLength(idAnoEscolarAluno,10);</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K19" s="10" t="str">
+        <f t="shared" ref="K19:K52" si="3">_xlfn.CONCAT("obj.set",H19,"(rs.getString(",$K$54,H19,$K$54,"));")</f>
+        <v>obj.setAnoEscolarAluno(rs.getString("AnoEscolarAluno"));</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="1"/>
+        <v>idAnoEscolarAluno.setText(aluno.getAnoEscolarAluno());</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -1423,22 +1663,30 @@
         <v>NomeMae varchar(60) NOT NULL ,</v>
       </c>
       <c r="G20" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C20,9,2)</f>
         <v>60</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>20</v>
       </c>
       <c r="I20" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E20,",obj.get",H20,"());")</f>
         <v>st.setString(19,obj.getNomeMae());</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H20,",",G20,");")</f>
         <v>Constraints.setTextFieldMaxLength(idNomeMae,60);</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K20" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setNomeMae(rs.getString("NomeMae"));</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="1"/>
+        <v>idNomeMae.setText(aluno.getNomeMae());</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1459,22 +1707,30 @@
         <v>RgMae varchar(15) NOT NULL ,</v>
       </c>
       <c r="G21" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C21,9,2)</f>
         <v>15</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>21</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E21,",obj.get",H21,"());")</f>
         <v>st.setString(20,obj.getRgMae());</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H21,",",G21,");")</f>
         <v>Constraints.setTextFieldMaxLength(idRgMae,15);</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K21" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setRgMae(rs.getString("RgMae"));</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="1"/>
+        <v>idRgMae.setText(aluno.getRgMae());</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -1495,22 +1751,30 @@
         <v>CpfMae varchar(15) NOT NULL ,</v>
       </c>
       <c r="G22" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C22,9,2)</f>
         <v>15</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>22</v>
       </c>
       <c r="I22" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E22,",obj.get",H22,"());")</f>
         <v>st.setString(21,obj.getCpfMae());</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H22,",",G22,");")</f>
         <v>Constraints.setTextFieldMaxLength(idCpfMae,15);</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K22" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setCpfMae(rs.getString("CpfMae"));</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="1"/>
+        <v>idCpfMae.setText(aluno.getCpfMae());</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -1531,22 +1795,30 @@
         <v>CelularMae varchar(15) NOT NULL ,</v>
       </c>
       <c r="G23" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C23,9,2)</f>
         <v>15</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>23</v>
       </c>
       <c r="I23" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E23,",obj.get",H23,"());")</f>
         <v>st.setString(22,obj.getCelularMae());</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H23,",",G23,");")</f>
         <v>Constraints.setTextFieldMaxLength(idCelularMae,15);</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K23" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setCelularMae(rs.getString("CelularMae"));</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="1"/>
+        <v>idCelularMae.setText(aluno.getCelularMae());</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -1567,22 +1839,30 @@
         <v>NomePai varchar(60)   ,</v>
       </c>
       <c r="G24" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C24,9,2)</f>
         <v>60</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>24</v>
       </c>
       <c r="I24" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E24,",obj.get",H24,"());")</f>
         <v>st.setString(23,obj.getNomePai());</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H24,",",G24,");")</f>
         <v>Constraints.setTextFieldMaxLength(idNomePai,60);</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K24" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setNomePai(rs.getString("NomePai"));</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="1"/>
+        <v>idNomePai.setText(aluno.getNomePai());</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -1603,22 +1883,30 @@
         <v>RgPai varchar(15)   ,</v>
       </c>
       <c r="G25" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C25,9,2)</f>
         <v>15</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>25</v>
       </c>
       <c r="I25" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E25,",obj.get",H25,"());")</f>
         <v>st.setString(24,obj.getRgPai());</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H25,",",G25,");")</f>
         <v>Constraints.setTextFieldMaxLength(idRgPai,15);</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K25" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setRgPai(rs.getString("RgPai"));</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="1"/>
+        <v>idRgPai.setText(aluno.getRgPai());</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1639,22 +1927,30 @@
         <v>CpfPai varchar(15)   ,</v>
       </c>
       <c r="G26" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C26,9,2)</f>
         <v>15</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>26</v>
       </c>
       <c r="I26" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E26,",obj.get",H26,"());")</f>
         <v>st.setString(25,obj.getCpfPai());</v>
       </c>
       <c r="J26" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H26,",",G26,");")</f>
         <v>Constraints.setTextFieldMaxLength(idCpfPai,15);</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K26" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setCpfPai(rs.getString("CpfPai"));</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="1"/>
+        <v>idCpfPai.setText(aluno.getCpfPai());</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -1675,22 +1971,30 @@
         <v>CelularPai varchar(15)   ,</v>
       </c>
       <c r="G27" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C27,9,2)</f>
         <v>15</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>27</v>
       </c>
       <c r="I27" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E27,",obj.get",H27,"());")</f>
         <v>st.setString(26,obj.getCelularPai());</v>
       </c>
       <c r="J27" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H27,",",G27,");")</f>
         <v>Constraints.setTextFieldMaxLength(idCelularPai,15);</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K27" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setCelularPai(rs.getString("CelularPai"));</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="1"/>
+        <v>idCelularPai.setText(aluno.getCelularPai());</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -1711,22 +2015,30 @@
         <v>NomeResponsavel varchar(60) NOT NULL ,</v>
       </c>
       <c r="G28" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C28,9,2)</f>
         <v>60</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>28</v>
       </c>
       <c r="I28" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E28,",obj.get",H28,"());")</f>
         <v>st.setString(27,obj.getNomeResponsavel());</v>
       </c>
       <c r="J28" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H28,",",G28,");")</f>
         <v>Constraints.setTextFieldMaxLength(idNomeResponsavel,60);</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K28" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setNomeResponsavel(rs.getString("NomeResponsavel"));</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="1"/>
+        <v>idNomeResponsavel.setText(aluno.getNomeResponsavel());</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -1747,22 +2059,30 @@
         <v>RgResponsavel varchar(20) NOT NULL ,</v>
       </c>
       <c r="G29" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C29,9,2)</f>
         <v>20</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>29</v>
       </c>
       <c r="I29" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E29,",obj.get",H29,"());")</f>
         <v>st.setString(28,obj.getRgResponsavel());</v>
       </c>
       <c r="J29" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H29,",",G29,");")</f>
         <v>Constraints.setTextFieldMaxLength(idRgResponsavel,20);</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K29" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setRgResponsavel(rs.getString("RgResponsavel"));</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="1"/>
+        <v>idRgResponsavel.setText(aluno.getRgResponsavel());</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -1783,22 +2103,30 @@
         <v>CpfResponsavel varchar(15) NOT NULL ,</v>
       </c>
       <c r="G30" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C30,9,2)</f>
         <v>15</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>30</v>
       </c>
       <c r="I30" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E30,",obj.get",H30,"());")</f>
         <v>st.setString(29,obj.getCpfResponsavel());</v>
       </c>
       <c r="J30" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H30,",",G30,");")</f>
         <v>Constraints.setTextFieldMaxLength(idCpfResponsavel,15);</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K30" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setCpfResponsavel(rs.getString("CpfResponsavel"));</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="1"/>
+        <v>idCpfResponsavel.setText(aluno.getCpfResponsavel());</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -1819,22 +2147,30 @@
         <v>CelularResponsavel varchar(15) NOT NULL ,</v>
       </c>
       <c r="G31" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C31,9,2)</f>
         <v>15</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>31</v>
       </c>
       <c r="I31" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E31,",obj.get",H31,"());")</f>
         <v>st.setString(30,obj.getCelularResponsavel());</v>
       </c>
       <c r="J31" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H31,",",G31,");")</f>
         <v>Constraints.setTextFieldMaxLength(idCelularResponsavel,15);</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K31" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setCelularResponsavel(rs.getString("CelularResponsavel"));</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="1"/>
+        <v>idCelularResponsavel.setText(aluno.getCelularResponsavel());</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -1855,22 +2191,30 @@
         <v>EnderecoTrabalho varchar(60)   ,</v>
       </c>
       <c r="G32" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C32,9,2)</f>
         <v>60</v>
       </c>
       <c r="H32" s="6" t="s">
         <v>33</v>
       </c>
       <c r="I32" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E32,",obj.get",H32,"());")</f>
         <v>st.setString(31,obj.getEnderecoTrabalho());</v>
       </c>
       <c r="J32" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H32,",",G32,");")</f>
         <v>Constraints.setTextFieldMaxLength(idEnderecoTrabalho,60);</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K32" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setEnderecoTrabalho(rs.getString("EnderecoTrabalho"));</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="1"/>
+        <v>idEnderecoTrabalho.setText(aluno.getEnderecoTrabalho());</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -1878,7 +2222,7 @@
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D33" t="s">
         <v>65</v>
@@ -1897,15 +2241,23 @@
         <v>32</v>
       </c>
       <c r="I33" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E33,",obj.get",H33,"());")</f>
         <v>st.setString(32,obj.getNumeroTrabalho());</v>
       </c>
       <c r="J33" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H33,",",G33,");")</f>
         <v>Constraints.setTextFieldMaxLength(idNumeroTrabalho,4);</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K33" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setNumeroTrabalho(rs.getString("NumeroTrabalho"));</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="1"/>
+        <v>idNumeroTrabalho.setText(aluno.getNumeroTrabalho());</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -1926,22 +2278,30 @@
         <v>CepTrabalho varchar(20)   ,</v>
       </c>
       <c r="G34" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C34,9,2)</f>
         <v>20</v>
       </c>
       <c r="H34" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I34" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E34,",obj.get",H34,"());")</f>
         <v>st.setString(33,obj.getCepTrabalho());</v>
       </c>
       <c r="J34" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H34,",",G34,");")</f>
         <v>Constraints.setTextFieldMaxLength(idCepTrabalho,20);</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K34" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setCepTrabalho(rs.getString("CepTrabalho"));</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="1"/>
+        <v>idCepTrabalho.setText(aluno.getCepTrabalho());</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -1962,22 +2322,30 @@
         <v>Moradia varchar(12) NOT NULL ,</v>
       </c>
       <c r="G35" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C35,9,2)</f>
         <v>12</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>35</v>
       </c>
       <c r="I35" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E35,",obj.get",H35,"());")</f>
         <v>st.setString(34,obj.getMoradia());</v>
       </c>
       <c r="J35" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H35,",",G35,");")</f>
         <v>Constraints.setTextFieldMaxLength(idMoradia,12);</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K35" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setMoradia(rs.getString("Moradia"));</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="1"/>
+        <v>idMoradia.setText(aluno.getMoradia());</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -1985,7 +2353,7 @@
         <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D36" t="s">
         <v>53</v>
@@ -2004,15 +2372,23 @@
         <v>36</v>
       </c>
       <c r="I36" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E36,",obj.get",H36,"());")</f>
         <v>st.setString(35,obj.getNumeroPessoasNaMoradia());</v>
       </c>
       <c r="J36" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H36,",",G36,");")</f>
         <v>Constraints.setTextFieldMaxLength(idNumeroPessoasNaMoradia,2);</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K36" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setNumeroPessoasNaMoradia(rs.getString("NumeroPessoasNaMoradia"));</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="1"/>
+        <v>idNumeroPessoasNaMoradia.setText(aluno.getNumeroPessoasNaMoradia());</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -2020,7 +2396,7 @@
         <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D37" t="s">
         <v>53</v>
@@ -2033,22 +2409,30 @@
         <v>Alergia varchar(04) NOT NULL ,</v>
       </c>
       <c r="G37" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C37,9,2)</f>
         <v>04</v>
       </c>
       <c r="H37" s="6" t="s">
         <v>37</v>
       </c>
       <c r="I37" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E37,",obj.get",H37,"());")</f>
         <v>st.setString(36,obj.getAlergia());</v>
       </c>
       <c r="J37" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H37,",",G37,");")</f>
         <v>Constraints.setTextFieldMaxLength(idAlergia,04);</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K37" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setAlergia(rs.getString("Alergia"));</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="1"/>
+        <v>idAlergia.setText(aluno.getAlergia());</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -2069,22 +2453,30 @@
         <v>AlergiaQual varchar(60)   ,</v>
       </c>
       <c r="G38" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C38,9,2)</f>
         <v>60</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>38</v>
       </c>
       <c r="I38" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E38,",obj.get",H38,"());")</f>
         <v>st.setString(37,obj.getAlergiaQual());</v>
       </c>
       <c r="J38" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H38,",",G38,");")</f>
         <v>Constraints.setTextFieldMaxLength(idAlergiaQual,60);</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K38" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setAlergiaQual(rs.getString("AlergiaQual"));</v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="1"/>
+        <v>idAlergiaQual.setText(aluno.getAlergiaQual());</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -2092,7 +2484,7 @@
         <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D39" t="s">
         <v>53</v>
@@ -2105,22 +2497,30 @@
         <v>Deficiencia varchar(04) NOT NULL ,</v>
       </c>
       <c r="G39" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C39,9,2)</f>
         <v>04</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>39</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E39,",obj.get",H39,"());")</f>
         <v>st.setString(38,obj.getDeficiencia());</v>
       </c>
       <c r="J39" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H39,",",G39,");")</f>
         <v>Constraints.setTextFieldMaxLength(idDeficiencia,04);</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K39" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setDeficiencia(rs.getString("Deficiencia"));</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="1"/>
+        <v>idDeficiencia.setText(aluno.getDeficiencia());</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -2141,22 +2541,30 @@
         <v>DeficienciaQual varchar(60)   ,</v>
       </c>
       <c r="G40" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C40,9,2)</f>
         <v>60</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>40</v>
       </c>
       <c r="I40" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E40,",obj.get",H40,"());")</f>
         <v>st.setString(39,obj.getDeficienciaQual());</v>
       </c>
       <c r="J40" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H40,",",G40,");")</f>
         <v>Constraints.setTextFieldMaxLength(idDeficienciaQual,60);</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K40" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setDeficienciaQual(rs.getString("DeficienciaQual"));</v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="1"/>
+        <v>idDeficienciaQual.setText(aluno.getDeficienciaQual());</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -2164,7 +2572,7 @@
         <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D41" t="s">
         <v>53</v>
@@ -2177,22 +2585,30 @@
         <v>Cirurgia varchar(04) NOT NULL ,</v>
       </c>
       <c r="G41" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C41,9,2)</f>
         <v>04</v>
       </c>
       <c r="H41" s="6" t="s">
         <v>41</v>
       </c>
       <c r="I41" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E41,",obj.get",H41,"());")</f>
         <v>st.setString(40,obj.getCirurgia());</v>
       </c>
       <c r="J41" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H41,",",G41,");")</f>
         <v>Constraints.setTextFieldMaxLength(idCirurgia,04);</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K41" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setCirurgia(rs.getString("Cirurgia"));</v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="1"/>
+        <v>idCirurgia.setText(aluno.getCirurgia());</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -2213,22 +2629,30 @@
         <v>CirurgiaQual varchar(60)   ,</v>
       </c>
       <c r="G42" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C42,9,2)</f>
         <v>60</v>
       </c>
       <c r="H42" s="6" t="s">
         <v>42</v>
       </c>
       <c r="I42" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E42,",obj.get",H42,"());")</f>
         <v>st.setString(41,obj.getCirurgiaQual());</v>
       </c>
       <c r="J42" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H42,",",G42,");")</f>
         <v>Constraints.setTextFieldMaxLength(idCirurgiaQual,60);</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K42" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setCirurgiaQual(rs.getString("CirurgiaQual"));</v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" si="1"/>
+        <v>idCirurgiaQual.setText(aluno.getCirurgiaQual());</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -2236,7 +2660,7 @@
         <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D43" t="s">
         <v>53</v>
@@ -2249,22 +2673,30 @@
         <v>Doenca varchar(04) NOT NULL ,</v>
       </c>
       <c r="G43" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C43,9,2)</f>
         <v>04</v>
       </c>
       <c r="H43" s="6" t="s">
         <v>43</v>
       </c>
       <c r="I43" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E43,",obj.get",H43,"());")</f>
         <v>st.setString(42,obj.getDoenca());</v>
       </c>
       <c r="J43" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H43,",",G43,");")</f>
         <v>Constraints.setTextFieldMaxLength(idDoenca,04);</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K43" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setDoenca(rs.getString("Doenca"));</v>
+      </c>
+      <c r="L43" t="str">
+        <f t="shared" si="1"/>
+        <v>idDoenca.setText(aluno.getDoenca());</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -2285,22 +2717,30 @@
         <v>DoencaQual varchar(60)   ,</v>
       </c>
       <c r="G44" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C44,9,2)</f>
         <v>60</v>
       </c>
       <c r="H44" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I44" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E44,",obj.get",H44,"());")</f>
         <v>st.setString(43,obj.getDoencaQual());</v>
       </c>
       <c r="J44" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H44,",",G44,");")</f>
         <v>Constraints.setTextFieldMaxLength(idDoencaQual,60);</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K44" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setDoencaQual(rs.getString("DoencaQual"));</v>
+      </c>
+      <c r="L44" t="str">
+        <f t="shared" si="1"/>
+        <v>idDoencaQual.setText(aluno.getDoencaQual());</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -2308,7 +2748,7 @@
         <v>45</v>
       </c>
       <c r="C45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D45" t="s">
         <v>53</v>
@@ -2321,22 +2761,30 @@
         <v>Remedio varchar(04) NOT NULL ,</v>
       </c>
       <c r="G45" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C45,9,2)</f>
         <v>04</v>
       </c>
       <c r="H45" s="6" t="s">
         <v>45</v>
       </c>
       <c r="I45" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E45,",obj.get",H45,"());")</f>
         <v>st.setString(44,obj.getRemedio());</v>
       </c>
       <c r="J45" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H45,",",G45,");")</f>
         <v>Constraints.setTextFieldMaxLength(idRemedio,04);</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K45" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setRemedio(rs.getString("Remedio"));</v>
+      </c>
+      <c r="L45" t="str">
+        <f t="shared" si="1"/>
+        <v>idRemedio.setText(aluno.getRemedio());</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -2357,22 +2805,30 @@
         <v>RemedioQual varchar(60)   ,</v>
       </c>
       <c r="G46" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C46,9,2)</f>
         <v>60</v>
       </c>
       <c r="H46" s="6" t="s">
         <v>46</v>
       </c>
       <c r="I46" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E46,",obj.get",H46,"());")</f>
         <v>st.setString(45,obj.getRemedioQual());</v>
       </c>
       <c r="J46" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H46,",",G46,");")</f>
         <v>Constraints.setTextFieldMaxLength(idRemedioQual,60);</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K46" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setRemedioQual(rs.getString("RemedioQual"));</v>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="1"/>
+        <v>idRemedioQual.setText(aluno.getRemedioQual());</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -2380,7 +2836,7 @@
         <v>47</v>
       </c>
       <c r="C47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D47" t="s">
         <v>53</v>
@@ -2393,22 +2849,30 @@
         <v>BolsaFamilia varchar(04) NOT NULL ,</v>
       </c>
       <c r="G47" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C47,9,2)</f>
         <v>04</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>47</v>
       </c>
       <c r="I47" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E47,",obj.get",H47,"());")</f>
         <v>st.setString(46,obj.getBolsaFamilia());</v>
       </c>
       <c r="J47" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H47,",",G47,");")</f>
         <v>Constraints.setTextFieldMaxLength(idBolsaFamilia,04);</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K47" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setBolsaFamilia(rs.getString("BolsaFamilia"));</v>
+      </c>
+      <c r="L47" t="str">
+        <f t="shared" si="1"/>
+        <v>idBolsaFamilia.setText(aluno.getBolsaFamilia());</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>2</v>
       </c>
@@ -2416,7 +2880,7 @@
         <v>48</v>
       </c>
       <c r="C48" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D48" t="s">
         <v>53</v>
@@ -2429,22 +2893,30 @@
         <v>Beneficio varchar(04) NOT NULL ,</v>
       </c>
       <c r="G48" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C48,9,2)</f>
         <v>04</v>
       </c>
       <c r="H48" s="6" t="s">
         <v>48</v>
       </c>
       <c r="I48" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E48,",obj.get",H48,"());")</f>
         <v>st.setString(47,obj.getBeneficio());</v>
       </c>
       <c r="J48" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H48,",",G48,");")</f>
         <v>Constraints.setTextFieldMaxLength(idBeneficio,04);</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K48" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setBeneficio(rs.getString("Beneficio"));</v>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="1"/>
+        <v>idBeneficio.setText(aluno.getBeneficio());</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -2452,7 +2924,7 @@
         <v>49</v>
       </c>
       <c r="C49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D49" t="s">
         <v>53</v>
@@ -2465,22 +2937,30 @@
         <v>CadastroUnico varchar(04) NOT NULL ,</v>
       </c>
       <c r="G49" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C49,9,2)</f>
         <v>04</v>
       </c>
       <c r="H49" s="6" t="s">
         <v>49</v>
       </c>
       <c r="I49" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E49,",obj.get",H49,"());")</f>
         <v>st.setString(48,obj.getCadastroUnico());</v>
       </c>
       <c r="J49" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H49,",",G49,");")</f>
         <v>Constraints.setTextFieldMaxLength(idCadastroUnico,04);</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K49" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setCadastroUnico(rs.getString("CadastroUnico"));</v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" si="1"/>
+        <v>idCadastroUnico.setText(aluno.getCadastroUnico());</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -2507,15 +2987,23 @@
         <v>70</v>
       </c>
       <c r="I50" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E50,",obj.get",H50,"());")</f>
         <v>st.setString(49,obj.getNumeroNIS());</v>
       </c>
       <c r="J50" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H50,",",G50,");")</f>
         <v>Constraints.setTextFieldMaxLength(idNumeroNIS,11);</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K50" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setNumeroNIS(rs.getString("NumeroNIS"));</v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="1"/>
+        <v>idNumeroNIS.setText(aluno.getNumeroNIS());</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>2</v>
       </c>
@@ -2536,22 +3024,30 @@
         <v>Encaminha varchar(20) NOT NULL ,</v>
       </c>
       <c r="G51" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C51,9,2)</f>
         <v>20</v>
       </c>
       <c r="H51" s="6" t="s">
         <v>50</v>
       </c>
       <c r="I51" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("st.setString(",E51,",obj.get",H51,"());")</f>
         <v>st.setString(50,obj.getEncaminha());</v>
       </c>
       <c r="J51" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H51,",",G51,");")</f>
         <v>Constraints.setTextFieldMaxLength(idEncaminha,20);</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K51" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setEncaminha(rs.getString("Encaminha"));</v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="1"/>
+        <v>idEncaminha.setText(aluno.getEncaminha());</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -2569,72 +3065,86 @@
         <v>EncaminhaOutra varchar(60)  ,</v>
       </c>
       <c r="G52" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(C52,9,2)</f>
         <v>60</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="I52" t="str">
-        <f t="shared" si="2"/>
-        <v>st.setString(51,obj.getEncaminhaOutra)());</v>
+        <f>_xlfn.CONCAT("st.setString(",E52,",obj.get",H52,"());")</f>
+        <v>st.setString(51,obj.getEncaminhaOutra());</v>
       </c>
       <c r="J52" t="str">
-        <f t="shared" si="0"/>
-        <v>Constraints.setTextFieldMaxLength(idEncaminhaOutra),60);</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H52,",",G52,");")</f>
+        <v>Constraints.setTextFieldMaxLength(idEncaminhaOutra,60);</v>
+      </c>
+      <c r="K52" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>obj.setEncaminhaOutra(rs.getString("EncaminhaOutra"));</v>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="1"/>
+        <v>idEncaminhaOutra.setText(aluno.getEncaminhaOutra());</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F53" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K54" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I61" s="11"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
         <v>53</v>
       </c>
@@ -2846,4 +3356,685 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA6A3C9-69F0-4CB1-982B-4B74265FEC2E}">
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="26.28515625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18">
+        <v>1</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="16" t="str">
+        <f>_xlfn.CONCAT(B1,"=?, ")</f>
+        <v xml:space="preserve">NomeAluno=?, </v>
+      </c>
+      <c r="D1" t="str">
+        <f>_xlfn.CONCAT(C1:C50)</f>
+        <v xml:space="preserve">NomeAluno=?, DataCadastro=?, Situacao=?, RgAluno=?, CpfAluno=?, DataNascimentoAluno=?, Sexo=?, NomeRuaAluno=?, NumeroRuaAluno=?, BairroAluno=?, CepAluno=?, CelularAluno=?, TelFixoAluno=?, EmailAluno=?, EscolaAluno=?, PeriodoAluno=?, AnoEscolarAluno=?, NomeMae=?, RgMae=?, CpfMae=?, CelularMae=?, NomePai=?, RgPai=?, CpfPai=?, CelularPai=?, NomeResponsavel=?, RgResponsavel=?, CpfResponsavel=?, CelularResponsavel=?, EnderecoTrabalho=?, NumeroTrabalho=?, CepTrabalho=?, Moradia=?, NumeroPessoasNaMoradia=?, Alergia=?, AlergiaQual=?, Deficiencia=?, DeficienciaQual=?, Cirurgia=?, CirurgiaQual=?, Doenca=?, DoencaQual=?, Remedio=?, RemedioQual=?, BolsaFamilia=?, Beneficio=?, CadastroUnico=?, NumeroNIS=?, Encaminha=?, EncaminhaOutra=?, </v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18">
+        <f>A1+1</f>
+        <v>2</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="16" t="str">
+        <f t="shared" ref="C2:C51" si="0">_xlfn.CONCAT(B2,"=?, ")</f>
+        <v xml:space="preserve">DataCadastro=?, </v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <f t="shared" ref="A3:A50" si="1">A2+1</f>
+        <v>3</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Situacao=?, </v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">RgAluno=?, </v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CpfAluno=?, </v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">DataNascimentoAluno=?, </v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Sexo=?, </v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">NomeRuaAluno=?, </v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">NumeroRuaAluno=?, </v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">BairroAluno=?, </v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CepAluno=?, </v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CelularAluno=?, </v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">TelFixoAluno=?, </v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EmailAluno=?, </v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EscolaAluno=?, </v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">PeriodoAluno=?, </v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">AnoEscolarAluno=?, </v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">NomeMae=?, </v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="18">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">RgMae=?, </v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="18">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CpfMae=?, </v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CelularMae=?, </v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">NomePai=?, </v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">RgPai=?, </v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CpfPai=?, </v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CelularPai=?, </v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="18">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">NomeResponsavel=?, </v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="18">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">RgResponsavel=?, </v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="18">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CpfResponsavel=?, </v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="18">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CelularResponsavel=?, </v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="18">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EnderecoTrabalho=?, </v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="18">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">NumeroTrabalho=?, </v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="18">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CepTrabalho=?, </v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Moradia=?, </v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="18">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">NumeroPessoasNaMoradia=?, </v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="18">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Alergia=?, </v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="18">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">AlergiaQual=?, </v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="18">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Deficiencia=?, </v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="18">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">DeficienciaQual=?, </v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="18">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Cirurgia=?, </v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="18">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CirurgiaQual=?, </v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="18">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Doenca=?, </v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="18">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">DoencaQual=?, </v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="18">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Remedio=?, </v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="18">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">RemedioQual=?, </v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="18">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">BolsaFamilia=?, </v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="18">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Beneficio=?, </v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="18">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CadastroUnico=?, </v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="18">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">NumeroNIS=?, </v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="18">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Encaminha=?, </v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="18">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EncaminhaOutra=?, </v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="13"/>
+      <c r="C51" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">=?, </v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Antes de mexer nas datas
</commit_message>
<xml_diff>
--- a/Tabela_Aluno_Campos.xlsx
+++ b/Tabela_Aluno_Campos.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jribe\eclipse-workspace\MariaLobatoGenteJovem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D764F363-A832-401C-9ED7-5169B657E3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAB0E5F-A505-4726-BFC9-D741E94753AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="1" xr2:uid="{BCEF3EA5-B1A7-48E7-889E-E8D820FE6D87}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{BCEF3EA5-B1A7-48E7-889E-E8D820FE6D87}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="CRIAR A TABELA" sheetId="3" r:id="rId2"/>
+    <sheet name="  " sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="OLE_LINK1" localSheetId="0">Planilha1!#REF!</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="90">
   <si>
     <t>Integer</t>
   </si>
@@ -277,6 +278,39 @@
   </si>
   <si>
     <t>INICIALIZA_FORMULARIO</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>DataMatricula</t>
+  </si>
+  <si>
+    <t>DataExclusao</t>
+  </si>
+  <si>
+    <t>TurmaRegular</t>
+  </si>
+  <si>
+    <t>TurmaEspecial</t>
+  </si>
+  <si>
+    <t>RendaFamiliar</t>
+  </si>
+  <si>
+    <t>CREATE TABLE aluno</t>
+  </si>
+  <si>
+    <t>(id int  NOT NULL  AUTO_INCREMENT ,</t>
+  </si>
+  <si>
+    <t>UNIQUE KEY(CpfAluno) ,</t>
+  </si>
+  <si>
+    <t>);</t>
+  </si>
+  <si>
+    <t>DATE</t>
   </si>
 </sst>
 </file>
@@ -798,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B5FD43-F609-42B4-90F4-71811082D573}">
   <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView topLeftCell="C45" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L52"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D52" sqref="C3:D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,7 +903,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="2" t="str">
-        <f t="shared" ref="F2:F33" si="0">_xlfn.CONCAT(B2," ",C2," ",D2," ,")</f>
+        <f t="shared" ref="F2" si="0">_xlfn.CONCAT(B2," ",C2," ",D2," ,")</f>
         <v>id int(11)  NOT NULL  AUTO_INCREMENT ,</v>
       </c>
       <c r="G2" s="9">
@@ -879,11 +913,11 @@
         <v>1</v>
       </c>
       <c r="I2" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E2,",obj.get",H2,"());")</f>
+        <f t="shared" ref="I2:I33" si="1">_xlfn.CONCAT("st.setString(",E2,",obj.get",H2,"());")</f>
         <v>st.setString(1,obj.getid());</v>
       </c>
       <c r="J2" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H2,",",G2,");")</f>
+        <f t="shared" ref="J2:J33" si="2">_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H2,",",G2,");")</f>
         <v>Constraints.setTextFieldMaxLength(idid,11);</v>
       </c>
       <c r="K2" s="10" t="str">
@@ -912,22 +946,22 @@
         <v>2</v>
       </c>
       <c r="F3" s="2" t="str">
-        <f>_xlfn.CONCAT(B3," ",C3," ",D3," ,")</f>
+        <f t="shared" ref="F3:F34" si="3">_xlfn.CONCAT(B3," ",C3," ",D3," ,")</f>
         <v>NomeAluno varchar(60) NOT NULL ,</v>
       </c>
       <c r="G3" s="9" t="str">
-        <f>MID(C3,9,2)</f>
+        <f t="shared" ref="G3:G10" si="4">MID(C3,9,2)</f>
         <v>60</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="I3" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E3,",obj.get",H3,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(2,obj.getNomeAluno());</v>
       </c>
       <c r="J3" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H3,",",G3,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idNomeAluno,60);</v>
       </c>
       <c r="K3" s="10" t="str">
@@ -935,7 +969,7 @@
         <v>obj.setNomeAluno(rs.getString("NomeAluno"));</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:L52" si="1">_xlfn.CONCAT("id",H3,".setText(aluno.get",H3,"());")</f>
+        <f t="shared" ref="L3:L52" si="5">_xlfn.CONCAT("id",H3,".setText(aluno.get",H3,"());")</f>
         <v>idNomeAluno.setText(aluno.getNomeAluno());</v>
       </c>
     </row>
@@ -956,30 +990,30 @@
         <v>3</v>
       </c>
       <c r="F4" s="2" t="str">
-        <f>_xlfn.CONCAT(B4," ",C4," ",D4," ,")</f>
+        <f t="shared" si="3"/>
         <v>DataCadastro varchar(10) NOT NULL ,</v>
       </c>
       <c r="G4" s="9" t="str">
-        <f>MID(C4,9,2)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="I4" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E4,",obj.get",H4,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(3,obj.getDataCadastro());</v>
       </c>
       <c r="J4" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H4,",",G4,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idDataCadastro,10);</v>
       </c>
       <c r="K4" s="10" t="str">
-        <f t="shared" ref="K4:K16" si="2">_xlfn.CONCAT("obj.set",H4,"(rs.getString(",$K$54,H4,$K$54,"));")</f>
+        <f t="shared" ref="K4:K16" si="6">_xlfn.CONCAT("obj.set",H4,"(rs.getString(",$K$54,H4,$K$54,"));")</f>
         <v>obj.setDataCadastro(rs.getString("DataCadastro"));</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idDataCadastro.setText(aluno.getDataCadastro());</v>
       </c>
     </row>
@@ -1000,30 +1034,30 @@
         <v>4</v>
       </c>
       <c r="F5" s="2" t="str">
-        <f>_xlfn.CONCAT(B5," ",C5," ",D5," ,")</f>
+        <f t="shared" si="3"/>
         <v>Situacao varchar(10) NOT NULL ,</v>
       </c>
       <c r="G5" s="9" t="str">
-        <f>MID(C5,9,2)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="I5" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E5,",obj.get",H5,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(4,obj.getSituacao());</v>
       </c>
       <c r="J5" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H5,",",G5,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idSituacao,10);</v>
       </c>
       <c r="K5" s="10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>obj.setSituacao(rs.getString("Situacao"));</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idSituacao.setText(aluno.getSituacao());</v>
       </c>
     </row>
@@ -1044,30 +1078,30 @@
         <v>5</v>
       </c>
       <c r="F6" s="2" t="str">
-        <f>_xlfn.CONCAT(B6," ",C6," ",D6," ,")</f>
+        <f t="shared" si="3"/>
         <v>RgAluno varchar(15) NOT NULL ,</v>
       </c>
       <c r="G6" s="9" t="str">
-        <f>MID(C6,9,2)</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="I6" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E6,",obj.get",H6,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(5,obj.getRgAluno());</v>
       </c>
       <c r="J6" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H6,",",G6,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idRgAluno,15);</v>
       </c>
       <c r="K6" s="10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>obj.setRgAluno(rs.getString("RgAluno"));</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idRgAluno.setText(aluno.getRgAluno());</v>
       </c>
     </row>
@@ -1088,30 +1122,30 @@
         <v>6</v>
       </c>
       <c r="F7" s="2" t="str">
-        <f>_xlfn.CONCAT(B7," ",C7," ",D7," ,")</f>
+        <f t="shared" si="3"/>
         <v>CpfAluno varchar(15)   ,</v>
       </c>
       <c r="G7" s="9" t="str">
-        <f>MID(C7,9,2)</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I7" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E7,",obj.get",H7,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(6,obj.getCpfAluno());</v>
       </c>
       <c r="J7" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H7,",",G7,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idCpfAluno,15);</v>
       </c>
       <c r="K7" s="10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>obj.setCpfAluno(rs.getString("CpfAluno"));</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idCpfAluno.setText(aluno.getCpfAluno());</v>
       </c>
     </row>
@@ -1132,30 +1166,30 @@
         <v>7</v>
       </c>
       <c r="F8" s="2" t="str">
-        <f>_xlfn.CONCAT(B8," ",C8," ",D8," ,")</f>
+        <f t="shared" si="3"/>
         <v>DataNascimentoAluno varchar(10) NOT NULL ,</v>
       </c>
       <c r="G8" s="9" t="str">
-        <f>MID(C8,9,2)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="I8" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E8,",obj.get",H8,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(7,obj.getDataNascimentoAluno());</v>
       </c>
       <c r="J8" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H8,",",G8,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idDataNascimentoAluno,10);</v>
       </c>
       <c r="K8" s="10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>obj.setDataNascimentoAluno(rs.getString("DataNascimentoAluno"));</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idDataNascimentoAluno.setText(aluno.getDataNascimentoAluno());</v>
       </c>
     </row>
@@ -1176,30 +1210,30 @@
         <v>8</v>
       </c>
       <c r="F9" s="2" t="str">
-        <f>_xlfn.CONCAT(B9," ",C9," ",D9," ,")</f>
+        <f t="shared" si="3"/>
         <v>Sexo varchar(13) NOT NULL ,</v>
       </c>
       <c r="G9" s="9" t="str">
-        <f>MID(C9,9,2)</f>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="I9" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E9,",obj.get",H9,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(8,obj.getSexo());</v>
       </c>
       <c r="J9" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H9,",",G9,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idSexo,13);</v>
       </c>
       <c r="K9" s="10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>obj.setSexo(rs.getString("Sexo"));</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idSexo.setText(aluno.getSexo());</v>
       </c>
     </row>
@@ -1220,30 +1254,30 @@
         <v>9</v>
       </c>
       <c r="F10" s="2" t="str">
-        <f>_xlfn.CONCAT(B10," ",C10," ",D10," ,")</f>
+        <f t="shared" si="3"/>
         <v>NomeRuaAluno varchar(100) NOT NULL ,</v>
       </c>
       <c r="G10" s="9" t="str">
-        <f>MID(C10,9,2)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="I10" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E10,",obj.get",H10,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(9,obj.getNomeRuaAluno());</v>
       </c>
       <c r="J10" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H10,",",G10,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idNomeRuaAluno,10);</v>
       </c>
       <c r="K10" s="10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>obj.setNomeRuaAluno(rs.getString("NomeRuaAluno"));</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idNomeRuaAluno.setText(aluno.getNomeRuaAluno());</v>
       </c>
     </row>
@@ -1264,7 +1298,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="2" t="str">
-        <f>_xlfn.CONCAT(B11," ",C11," ",D11," ,")</f>
+        <f t="shared" si="3"/>
         <v>NumeroRuaAluno int(04) NOT NULL ,</v>
       </c>
       <c r="G11" s="9">
@@ -1274,19 +1308,19 @@
         <v>11</v>
       </c>
       <c r="I11" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E11,",obj.get",H11,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(10,obj.getNumeroRuaAluno());</v>
       </c>
       <c r="J11" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H11,",",G11,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idNumeroRuaAluno,4);</v>
       </c>
       <c r="K11" s="10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>obj.setNumeroRuaAluno(rs.getString("NumeroRuaAluno"));</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idNumeroRuaAluno.setText(aluno.getNumeroRuaAluno());</v>
       </c>
     </row>
@@ -1307,30 +1341,30 @@
         <v>11</v>
       </c>
       <c r="F12" s="2" t="str">
-        <f>_xlfn.CONCAT(B12," ",C12," ",D12," ,")</f>
+        <f t="shared" si="3"/>
         <v>BairroAluno varchar(60) NOT NULL ,</v>
       </c>
       <c r="G12" s="9" t="str">
-        <f>MID(C12,9,2)</f>
+        <f t="shared" ref="G12:G32" si="7">MID(C12,9,2)</f>
         <v>60</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I12" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E12,",obj.get",H12,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(11,obj.getBairroAluno());</v>
       </c>
       <c r="J12" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H12,",",G12,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idBairroAluno,60);</v>
       </c>
       <c r="K12" s="10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>obj.setBairroAluno(rs.getString("BairroAluno"));</v>
       </c>
       <c r="L12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idBairroAluno.setText(aluno.getBairroAluno());</v>
       </c>
     </row>
@@ -1351,30 +1385,30 @@
         <v>12</v>
       </c>
       <c r="F13" s="2" t="str">
-        <f>_xlfn.CONCAT(B13," ",C13," ",D13," ,")</f>
+        <f t="shared" si="3"/>
         <v>CepAluno varchar(20) NOT NULL ,</v>
       </c>
       <c r="G13" s="9" t="str">
-        <f>MID(C13,9,2)</f>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I13" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E13,",obj.get",H13,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(12,obj.getCepAluno());</v>
       </c>
       <c r="J13" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H13,",",G13,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idCepAluno,20);</v>
       </c>
       <c r="K13" s="10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>obj.setCepAluno(rs.getString("CepAluno"));</v>
       </c>
       <c r="L13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idCepAluno.setText(aluno.getCepAluno());</v>
       </c>
     </row>
@@ -1395,30 +1429,30 @@
         <v>13</v>
       </c>
       <c r="F14" s="2" t="str">
-        <f>_xlfn.CONCAT(B14," ",C14," ",D14," ,")</f>
+        <f t="shared" si="3"/>
         <v>CelularAluno varchar(15)   ,</v>
       </c>
       <c r="G14" s="9" t="str">
-        <f>MID(C14,9,2)</f>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I14" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E14,",obj.get",H14,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(13,obj.getCelularAluno());</v>
       </c>
       <c r="J14" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H14,",",G14,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idCelularAluno,15);</v>
       </c>
       <c r="K14" s="10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>obj.setCelularAluno(rs.getString("CelularAluno"));</v>
       </c>
       <c r="L14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idCelularAluno.setText(aluno.getCelularAluno());</v>
       </c>
     </row>
@@ -1439,30 +1473,30 @@
         <v>14</v>
       </c>
       <c r="F15" s="2" t="str">
-        <f>_xlfn.CONCAT(B15," ",C15," ",D15," ,")</f>
+        <f t="shared" si="3"/>
         <v>TelFixoAluno varchar(20)   ,</v>
       </c>
       <c r="G15" s="9" t="str">
-        <f>MID(C15,9,2)</f>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I15" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E15,",obj.get",H15,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(14,obj.getTelFixoAluno());</v>
       </c>
       <c r="J15" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H15,",",G15,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idTelFixoAluno,20);</v>
       </c>
       <c r="K15" s="10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>obj.setTelFixoAluno(rs.getString("TelFixoAluno"));</v>
       </c>
       <c r="L15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idTelFixoAluno.setText(aluno.getTelFixoAluno());</v>
       </c>
     </row>
@@ -1483,30 +1517,30 @@
         <v>15</v>
       </c>
       <c r="F16" s="2" t="str">
-        <f>_xlfn.CONCAT(B16," ",C16," ",D16," ,")</f>
+        <f t="shared" si="3"/>
         <v>EmailAluno varchar(60)   ,</v>
       </c>
       <c r="G16" s="9" t="str">
-        <f>MID(C16,9,2)</f>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="I16" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E16,",obj.get",H16,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(15,obj.getEmailAluno());</v>
       </c>
       <c r="J16" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H16,",",G16,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idEmailAluno,60);</v>
       </c>
       <c r="K16" s="10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>obj.setEmailAluno(rs.getString("EmailAluno"));</v>
       </c>
       <c r="L16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idEmailAluno.setText(aluno.getEmailAluno());</v>
       </c>
     </row>
@@ -1527,22 +1561,22 @@
         <v>16</v>
       </c>
       <c r="F17" s="2" t="str">
-        <f>_xlfn.CONCAT(B17," ",C17," ",D17," ,")</f>
+        <f t="shared" si="3"/>
         <v>EscolaAluno varchar(60) NOT NULL ,</v>
       </c>
       <c r="G17" s="9" t="str">
-        <f>MID(C17,9,2)</f>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I17" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E17,",obj.get",H17,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(16,obj.getEscolaAluno());</v>
       </c>
       <c r="J17" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H17,",",G17,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idEscolaAluno,60);</v>
       </c>
       <c r="K17" s="10" t="str">
@@ -1550,7 +1584,7 @@
         <v>obj.setEscolaAluno(rs.getString("EscolaAluno"));</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idEscolaAluno.setText(aluno.getEscolaAluno());</v>
       </c>
     </row>
@@ -1571,22 +1605,22 @@
         <v>17</v>
       </c>
       <c r="F18" s="2" t="str">
-        <f>_xlfn.CONCAT(B18," ",C18," ",D18," ,")</f>
+        <f t="shared" si="3"/>
         <v>PeriodoAluno varchar(10) NOT NULL ,</v>
       </c>
       <c r="G18" s="9" t="str">
-        <f>MID(C18,9,2)</f>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>18</v>
       </c>
       <c r="I18" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E18,",obj.get",H18,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(17,obj.getPeriodoAluno());</v>
       </c>
       <c r="J18" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H18,",",G18,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idPeriodoAluno,10);</v>
       </c>
       <c r="K18" s="10" t="str">
@@ -1594,7 +1628,7 @@
         <v>obj.setPeriodoAluno(rs.getString("PeriodoAluno"));</v>
       </c>
       <c r="L18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idPeriodoAluno.setText(aluno.getPeriodoAluno());</v>
       </c>
     </row>
@@ -1615,30 +1649,30 @@
         <v>18</v>
       </c>
       <c r="F19" s="2" t="str">
-        <f>_xlfn.CONCAT(B19," ",C19," ",D19," ,")</f>
+        <f t="shared" si="3"/>
         <v>AnoEscolarAluno varchar(10) NOT NULL ,</v>
       </c>
       <c r="G19" s="9" t="str">
-        <f>MID(C19,9,2)</f>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>19</v>
       </c>
       <c r="I19" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E19,",obj.get",H19,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(18,obj.getAnoEscolarAluno());</v>
       </c>
       <c r="J19" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H19,",",G19,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idAnoEscolarAluno,10);</v>
       </c>
       <c r="K19" s="10" t="str">
-        <f t="shared" ref="K19:K52" si="3">_xlfn.CONCAT("obj.set",H19,"(rs.getString(",$K$54,H19,$K$54,"));")</f>
+        <f t="shared" ref="K19:K52" si="8">_xlfn.CONCAT("obj.set",H19,"(rs.getString(",$K$54,H19,$K$54,"));")</f>
         <v>obj.setAnoEscolarAluno(rs.getString("AnoEscolarAluno"));</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idAnoEscolarAluno.setText(aluno.getAnoEscolarAluno());</v>
       </c>
     </row>
@@ -1659,30 +1693,30 @@
         <v>19</v>
       </c>
       <c r="F20" s="2" t="str">
-        <f>_xlfn.CONCAT(B20," ",C20," ",D20," ,")</f>
+        <f t="shared" si="3"/>
         <v>NomeMae varchar(60) NOT NULL ,</v>
       </c>
       <c r="G20" s="9" t="str">
-        <f>MID(C20,9,2)</f>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>20</v>
       </c>
       <c r="I20" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E20,",obj.get",H20,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(19,obj.getNomeMae());</v>
       </c>
       <c r="J20" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H20,",",G20,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idNomeMae,60);</v>
       </c>
       <c r="K20" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setNomeMae(rs.getString("NomeMae"));</v>
       </c>
       <c r="L20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idNomeMae.setText(aluno.getNomeMae());</v>
       </c>
     </row>
@@ -1703,30 +1737,30 @@
         <v>20</v>
       </c>
       <c r="F21" s="2" t="str">
-        <f>_xlfn.CONCAT(B21," ",C21," ",D21," ,")</f>
+        <f t="shared" si="3"/>
         <v>RgMae varchar(15) NOT NULL ,</v>
       </c>
       <c r="G21" s="9" t="str">
-        <f>MID(C21,9,2)</f>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>21</v>
       </c>
       <c r="I21" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E21,",obj.get",H21,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(20,obj.getRgMae());</v>
       </c>
       <c r="J21" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H21,",",G21,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idRgMae,15);</v>
       </c>
       <c r="K21" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setRgMae(rs.getString("RgMae"));</v>
       </c>
       <c r="L21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idRgMae.setText(aluno.getRgMae());</v>
       </c>
     </row>
@@ -1747,30 +1781,30 @@
         <v>21</v>
       </c>
       <c r="F22" s="2" t="str">
-        <f>_xlfn.CONCAT(B22," ",C22," ",D22," ,")</f>
+        <f t="shared" si="3"/>
         <v>CpfMae varchar(15) NOT NULL ,</v>
       </c>
       <c r="G22" s="9" t="str">
-        <f>MID(C22,9,2)</f>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>22</v>
       </c>
       <c r="I22" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E22,",obj.get",H22,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(21,obj.getCpfMae());</v>
       </c>
       <c r="J22" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H22,",",G22,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idCpfMae,15);</v>
       </c>
       <c r="K22" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setCpfMae(rs.getString("CpfMae"));</v>
       </c>
       <c r="L22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idCpfMae.setText(aluno.getCpfMae());</v>
       </c>
     </row>
@@ -1791,30 +1825,30 @@
         <v>22</v>
       </c>
       <c r="F23" s="2" t="str">
-        <f>_xlfn.CONCAT(B23," ",C23," ",D23," ,")</f>
+        <f t="shared" si="3"/>
         <v>CelularMae varchar(15) NOT NULL ,</v>
       </c>
       <c r="G23" s="9" t="str">
-        <f>MID(C23,9,2)</f>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>23</v>
       </c>
       <c r="I23" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E23,",obj.get",H23,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(22,obj.getCelularMae());</v>
       </c>
       <c r="J23" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H23,",",G23,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idCelularMae,15);</v>
       </c>
       <c r="K23" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setCelularMae(rs.getString("CelularMae"));</v>
       </c>
       <c r="L23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idCelularMae.setText(aluno.getCelularMae());</v>
       </c>
     </row>
@@ -1835,30 +1869,30 @@
         <v>23</v>
       </c>
       <c r="F24" s="2" t="str">
-        <f>_xlfn.CONCAT(B24," ",C24," ",D24," ,")</f>
+        <f t="shared" si="3"/>
         <v>NomePai varchar(60)   ,</v>
       </c>
       <c r="G24" s="9" t="str">
-        <f>MID(C24,9,2)</f>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>24</v>
       </c>
       <c r="I24" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E24,",obj.get",H24,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(23,obj.getNomePai());</v>
       </c>
       <c r="J24" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H24,",",G24,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idNomePai,60);</v>
       </c>
       <c r="K24" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setNomePai(rs.getString("NomePai"));</v>
       </c>
       <c r="L24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idNomePai.setText(aluno.getNomePai());</v>
       </c>
     </row>
@@ -1879,30 +1913,30 @@
         <v>24</v>
       </c>
       <c r="F25" s="2" t="str">
-        <f>_xlfn.CONCAT(B25," ",C25," ",D25," ,")</f>
+        <f t="shared" si="3"/>
         <v>RgPai varchar(15)   ,</v>
       </c>
       <c r="G25" s="9" t="str">
-        <f>MID(C25,9,2)</f>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>25</v>
       </c>
       <c r="I25" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E25,",obj.get",H25,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(24,obj.getRgPai());</v>
       </c>
       <c r="J25" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H25,",",G25,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idRgPai,15);</v>
       </c>
       <c r="K25" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setRgPai(rs.getString("RgPai"));</v>
       </c>
       <c r="L25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idRgPai.setText(aluno.getRgPai());</v>
       </c>
     </row>
@@ -1923,30 +1957,30 @@
         <v>25</v>
       </c>
       <c r="F26" s="2" t="str">
-        <f>_xlfn.CONCAT(B26," ",C26," ",D26," ,")</f>
+        <f t="shared" si="3"/>
         <v>CpfPai varchar(15)   ,</v>
       </c>
       <c r="G26" s="9" t="str">
-        <f>MID(C26,9,2)</f>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>26</v>
       </c>
       <c r="I26" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E26,",obj.get",H26,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(25,obj.getCpfPai());</v>
       </c>
       <c r="J26" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H26,",",G26,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idCpfPai,15);</v>
       </c>
       <c r="K26" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setCpfPai(rs.getString("CpfPai"));</v>
       </c>
       <c r="L26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idCpfPai.setText(aluno.getCpfPai());</v>
       </c>
     </row>
@@ -1967,30 +2001,30 @@
         <v>26</v>
       </c>
       <c r="F27" s="2" t="str">
-        <f>_xlfn.CONCAT(B27," ",C27," ",D27," ,")</f>
+        <f t="shared" si="3"/>
         <v>CelularPai varchar(15)   ,</v>
       </c>
       <c r="G27" s="9" t="str">
-        <f>MID(C27,9,2)</f>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>27</v>
       </c>
       <c r="I27" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E27,",obj.get",H27,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(26,obj.getCelularPai());</v>
       </c>
       <c r="J27" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H27,",",G27,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idCelularPai,15);</v>
       </c>
       <c r="K27" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setCelularPai(rs.getString("CelularPai"));</v>
       </c>
       <c r="L27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idCelularPai.setText(aluno.getCelularPai());</v>
       </c>
     </row>
@@ -2011,30 +2045,30 @@
         <v>27</v>
       </c>
       <c r="F28" s="2" t="str">
-        <f>_xlfn.CONCAT(B28," ",C28," ",D28," ,")</f>
+        <f t="shared" si="3"/>
         <v>NomeResponsavel varchar(60) NOT NULL ,</v>
       </c>
       <c r="G28" s="9" t="str">
-        <f>MID(C28,9,2)</f>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>28</v>
       </c>
       <c r="I28" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E28,",obj.get",H28,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(27,obj.getNomeResponsavel());</v>
       </c>
       <c r="J28" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H28,",",G28,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idNomeResponsavel,60);</v>
       </c>
       <c r="K28" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setNomeResponsavel(rs.getString("NomeResponsavel"));</v>
       </c>
       <c r="L28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idNomeResponsavel.setText(aluno.getNomeResponsavel());</v>
       </c>
     </row>
@@ -2055,30 +2089,30 @@
         <v>28</v>
       </c>
       <c r="F29" s="2" t="str">
-        <f>_xlfn.CONCAT(B29," ",C29," ",D29," ,")</f>
+        <f t="shared" si="3"/>
         <v>RgResponsavel varchar(20) NOT NULL ,</v>
       </c>
       <c r="G29" s="9" t="str">
-        <f>MID(C29,9,2)</f>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>29</v>
       </c>
       <c r="I29" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E29,",obj.get",H29,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(28,obj.getRgResponsavel());</v>
       </c>
       <c r="J29" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H29,",",G29,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idRgResponsavel,20);</v>
       </c>
       <c r="K29" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setRgResponsavel(rs.getString("RgResponsavel"));</v>
       </c>
       <c r="L29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idRgResponsavel.setText(aluno.getRgResponsavel());</v>
       </c>
     </row>
@@ -2099,30 +2133,30 @@
         <v>29</v>
       </c>
       <c r="F30" s="2" t="str">
-        <f>_xlfn.CONCAT(B30," ",C30," ",D30," ,")</f>
+        <f t="shared" si="3"/>
         <v>CpfResponsavel varchar(15) NOT NULL ,</v>
       </c>
       <c r="G30" s="9" t="str">
-        <f>MID(C30,9,2)</f>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>30</v>
       </c>
       <c r="I30" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E30,",obj.get",H30,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(29,obj.getCpfResponsavel());</v>
       </c>
       <c r="J30" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H30,",",G30,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idCpfResponsavel,15);</v>
       </c>
       <c r="K30" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setCpfResponsavel(rs.getString("CpfResponsavel"));</v>
       </c>
       <c r="L30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idCpfResponsavel.setText(aluno.getCpfResponsavel());</v>
       </c>
     </row>
@@ -2143,30 +2177,30 @@
         <v>30</v>
       </c>
       <c r="F31" s="2" t="str">
-        <f>_xlfn.CONCAT(B31," ",C31," ",D31," ,")</f>
+        <f t="shared" si="3"/>
         <v>CelularResponsavel varchar(15) NOT NULL ,</v>
       </c>
       <c r="G31" s="9" t="str">
-        <f>MID(C31,9,2)</f>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>31</v>
       </c>
       <c r="I31" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E31,",obj.get",H31,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(30,obj.getCelularResponsavel());</v>
       </c>
       <c r="J31" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H31,",",G31,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idCelularResponsavel,15);</v>
       </c>
       <c r="K31" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setCelularResponsavel(rs.getString("CelularResponsavel"));</v>
       </c>
       <c r="L31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idCelularResponsavel.setText(aluno.getCelularResponsavel());</v>
       </c>
     </row>
@@ -2187,30 +2221,30 @@
         <v>31</v>
       </c>
       <c r="F32" s="2" t="str">
-        <f>_xlfn.CONCAT(B32," ",C32," ",D32," ,")</f>
+        <f t="shared" si="3"/>
         <v>EnderecoTrabalho varchar(60)   ,</v>
       </c>
       <c r="G32" s="9" t="str">
-        <f>MID(C32,9,2)</f>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="H32" s="6" t="s">
         <v>33</v>
       </c>
       <c r="I32" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E32,",obj.get",H32,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(31,obj.getEnderecoTrabalho());</v>
       </c>
       <c r="J32" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H32,",",G32,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idEnderecoTrabalho,60);</v>
       </c>
       <c r="K32" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setEnderecoTrabalho(rs.getString("EnderecoTrabalho"));</v>
       </c>
       <c r="L32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idEnderecoTrabalho.setText(aluno.getEnderecoTrabalho());</v>
       </c>
     </row>
@@ -2231,7 +2265,7 @@
         <v>32</v>
       </c>
       <c r="F33" s="2" t="str">
-        <f>_xlfn.CONCAT(B33," ",C33," ",D33," ,")</f>
+        <f t="shared" si="3"/>
         <v>NumeroTrabalho int(04)   ,</v>
       </c>
       <c r="G33" s="9">
@@ -2241,19 +2275,19 @@
         <v>32</v>
       </c>
       <c r="I33" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E33,",obj.get",H33,"());")</f>
+        <f t="shared" si="1"/>
         <v>st.setString(32,obj.getNumeroTrabalho());</v>
       </c>
       <c r="J33" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H33,",",G33,");")</f>
+        <f t="shared" si="2"/>
         <v>Constraints.setTextFieldMaxLength(idNumeroTrabalho,4);</v>
       </c>
       <c r="K33" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setNumeroTrabalho(rs.getString("NumeroTrabalho"));</v>
       </c>
       <c r="L33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idNumeroTrabalho.setText(aluno.getNumeroTrabalho());</v>
       </c>
     </row>
@@ -2274,7 +2308,7 @@
         <v>33</v>
       </c>
       <c r="F34" s="2" t="str">
-        <f>_xlfn.CONCAT(B34," ",C34," ",D34," ,")</f>
+        <f t="shared" si="3"/>
         <v>CepTrabalho varchar(20)   ,</v>
       </c>
       <c r="G34" s="9" t="str">
@@ -2285,19 +2319,19 @@
         <v>34</v>
       </c>
       <c r="I34" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E34,",obj.get",H34,"());")</f>
+        <f t="shared" ref="I34:I65" si="9">_xlfn.CONCAT("st.setString(",E34,",obj.get",H34,"());")</f>
         <v>st.setString(33,obj.getCepTrabalho());</v>
       </c>
       <c r="J34" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H34,",",G34,");")</f>
+        <f t="shared" ref="J34:J52" si="10">_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H34,",",G34,");")</f>
         <v>Constraints.setTextFieldMaxLength(idCepTrabalho,20);</v>
       </c>
       <c r="K34" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setCepTrabalho(rs.getString("CepTrabalho"));</v>
       </c>
       <c r="L34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idCepTrabalho.setText(aluno.getCepTrabalho());</v>
       </c>
     </row>
@@ -2318,7 +2352,7 @@
         <v>34</v>
       </c>
       <c r="F35" s="2" t="str">
-        <f>_xlfn.CONCAT(B35," ",C35," ",D35," ,")</f>
+        <f t="shared" ref="F35:F52" si="11">_xlfn.CONCAT(B35," ",C35," ",D35," ,")</f>
         <v>Moradia varchar(12) NOT NULL ,</v>
       </c>
       <c r="G35" s="9" t="str">
@@ -2329,19 +2363,19 @@
         <v>35</v>
       </c>
       <c r="I35" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E35,",obj.get",H35,"());")</f>
+        <f t="shared" si="9"/>
         <v>st.setString(34,obj.getMoradia());</v>
       </c>
       <c r="J35" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H35,",",G35,");")</f>
+        <f t="shared" si="10"/>
         <v>Constraints.setTextFieldMaxLength(idMoradia,12);</v>
       </c>
       <c r="K35" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setMoradia(rs.getString("Moradia"));</v>
       </c>
       <c r="L35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idMoradia.setText(aluno.getMoradia());</v>
       </c>
     </row>
@@ -2362,7 +2396,7 @@
         <v>35</v>
       </c>
       <c r="F36" s="2" t="str">
-        <f>_xlfn.CONCAT(B36," ",C36," ",D36," ,")</f>
+        <f t="shared" si="11"/>
         <v>NumeroPessoasNaMoradia int(02) NOT NULL ,</v>
       </c>
       <c r="G36" s="9">
@@ -2372,19 +2406,19 @@
         <v>36</v>
       </c>
       <c r="I36" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E36,",obj.get",H36,"());")</f>
+        <f t="shared" si="9"/>
         <v>st.setString(35,obj.getNumeroPessoasNaMoradia());</v>
       </c>
       <c r="J36" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H36,",",G36,");")</f>
+        <f t="shared" si="10"/>
         <v>Constraints.setTextFieldMaxLength(idNumeroPessoasNaMoradia,2);</v>
       </c>
       <c r="K36" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setNumeroPessoasNaMoradia(rs.getString("NumeroPessoasNaMoradia"));</v>
       </c>
       <c r="L36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idNumeroPessoasNaMoradia.setText(aluno.getNumeroPessoasNaMoradia());</v>
       </c>
     </row>
@@ -2405,30 +2439,30 @@
         <v>36</v>
       </c>
       <c r="F37" s="2" t="str">
-        <f>_xlfn.CONCAT(B37," ",C37," ",D37," ,")</f>
+        <f t="shared" si="11"/>
         <v>Alergia varchar(04) NOT NULL ,</v>
       </c>
       <c r="G37" s="9" t="str">
-        <f>MID(C37,9,2)</f>
+        <f t="shared" ref="G37:G49" si="12">MID(C37,9,2)</f>
         <v>04</v>
       </c>
       <c r="H37" s="6" t="s">
         <v>37</v>
       </c>
       <c r="I37" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E37,",obj.get",H37,"());")</f>
+        <f t="shared" si="9"/>
         <v>st.setString(36,obj.getAlergia());</v>
       </c>
       <c r="J37" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H37,",",G37,");")</f>
+        <f t="shared" si="10"/>
         <v>Constraints.setTextFieldMaxLength(idAlergia,04);</v>
       </c>
       <c r="K37" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setAlergia(rs.getString("Alergia"));</v>
       </c>
       <c r="L37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idAlergia.setText(aluno.getAlergia());</v>
       </c>
     </row>
@@ -2449,30 +2483,30 @@
         <v>37</v>
       </c>
       <c r="F38" s="2" t="str">
-        <f>_xlfn.CONCAT(B38," ",C38," ",D38," ,")</f>
+        <f t="shared" si="11"/>
         <v>AlergiaQual varchar(60)   ,</v>
       </c>
       <c r="G38" s="9" t="str">
-        <f>MID(C38,9,2)</f>
+        <f t="shared" si="12"/>
         <v>60</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>38</v>
       </c>
       <c r="I38" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E38,",obj.get",H38,"());")</f>
+        <f t="shared" si="9"/>
         <v>st.setString(37,obj.getAlergiaQual());</v>
       </c>
       <c r="J38" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H38,",",G38,");")</f>
+        <f t="shared" si="10"/>
         <v>Constraints.setTextFieldMaxLength(idAlergiaQual,60);</v>
       </c>
       <c r="K38" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setAlergiaQual(rs.getString("AlergiaQual"));</v>
       </c>
       <c r="L38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idAlergiaQual.setText(aluno.getAlergiaQual());</v>
       </c>
     </row>
@@ -2493,30 +2527,30 @@
         <v>38</v>
       </c>
       <c r="F39" s="2" t="str">
-        <f>_xlfn.CONCAT(B39," ",C39," ",D39," ,")</f>
+        <f t="shared" si="11"/>
         <v>Deficiencia varchar(04) NOT NULL ,</v>
       </c>
       <c r="G39" s="9" t="str">
-        <f>MID(C39,9,2)</f>
+        <f t="shared" si="12"/>
         <v>04</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>39</v>
       </c>
       <c r="I39" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E39,",obj.get",H39,"());")</f>
+        <f t="shared" si="9"/>
         <v>st.setString(38,obj.getDeficiencia());</v>
       </c>
       <c r="J39" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H39,",",G39,");")</f>
+        <f t="shared" si="10"/>
         <v>Constraints.setTextFieldMaxLength(idDeficiencia,04);</v>
       </c>
       <c r="K39" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setDeficiencia(rs.getString("Deficiencia"));</v>
       </c>
       <c r="L39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idDeficiencia.setText(aluno.getDeficiencia());</v>
       </c>
     </row>
@@ -2537,30 +2571,30 @@
         <v>39</v>
       </c>
       <c r="F40" s="2" t="str">
-        <f>_xlfn.CONCAT(B40," ",C40," ",D40," ,")</f>
+        <f t="shared" si="11"/>
         <v>DeficienciaQual varchar(60)   ,</v>
       </c>
       <c r="G40" s="9" t="str">
-        <f>MID(C40,9,2)</f>
+        <f t="shared" si="12"/>
         <v>60</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>40</v>
       </c>
       <c r="I40" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E40,",obj.get",H40,"());")</f>
+        <f t="shared" si="9"/>
         <v>st.setString(39,obj.getDeficienciaQual());</v>
       </c>
       <c r="J40" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H40,",",G40,");")</f>
+        <f t="shared" si="10"/>
         <v>Constraints.setTextFieldMaxLength(idDeficienciaQual,60);</v>
       </c>
       <c r="K40" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setDeficienciaQual(rs.getString("DeficienciaQual"));</v>
       </c>
       <c r="L40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idDeficienciaQual.setText(aluno.getDeficienciaQual());</v>
       </c>
     </row>
@@ -2581,30 +2615,30 @@
         <v>40</v>
       </c>
       <c r="F41" s="2" t="str">
-        <f>_xlfn.CONCAT(B41," ",C41," ",D41," ,")</f>
+        <f t="shared" si="11"/>
         <v>Cirurgia varchar(04) NOT NULL ,</v>
       </c>
       <c r="G41" s="9" t="str">
-        <f>MID(C41,9,2)</f>
+        <f t="shared" si="12"/>
         <v>04</v>
       </c>
       <c r="H41" s="6" t="s">
         <v>41</v>
       </c>
       <c r="I41" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E41,",obj.get",H41,"());")</f>
+        <f t="shared" si="9"/>
         <v>st.setString(40,obj.getCirurgia());</v>
       </c>
       <c r="J41" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H41,",",G41,");")</f>
+        <f t="shared" si="10"/>
         <v>Constraints.setTextFieldMaxLength(idCirurgia,04);</v>
       </c>
       <c r="K41" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setCirurgia(rs.getString("Cirurgia"));</v>
       </c>
       <c r="L41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idCirurgia.setText(aluno.getCirurgia());</v>
       </c>
     </row>
@@ -2625,30 +2659,30 @@
         <v>41</v>
       </c>
       <c r="F42" s="2" t="str">
-        <f>_xlfn.CONCAT(B42," ",C42," ",D42," ,")</f>
+        <f t="shared" si="11"/>
         <v>CirurgiaQual varchar(60)   ,</v>
       </c>
       <c r="G42" s="9" t="str">
-        <f>MID(C42,9,2)</f>
+        <f t="shared" si="12"/>
         <v>60</v>
       </c>
       <c r="H42" s="6" t="s">
         <v>42</v>
       </c>
       <c r="I42" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E42,",obj.get",H42,"());")</f>
+        <f t="shared" si="9"/>
         <v>st.setString(41,obj.getCirurgiaQual());</v>
       </c>
       <c r="J42" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H42,",",G42,");")</f>
+        <f t="shared" si="10"/>
         <v>Constraints.setTextFieldMaxLength(idCirurgiaQual,60);</v>
       </c>
       <c r="K42" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setCirurgiaQual(rs.getString("CirurgiaQual"));</v>
       </c>
       <c r="L42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idCirurgiaQual.setText(aluno.getCirurgiaQual());</v>
       </c>
     </row>
@@ -2669,30 +2703,30 @@
         <v>42</v>
       </c>
       <c r="F43" s="2" t="str">
-        <f>_xlfn.CONCAT(B43," ",C43," ",D43," ,")</f>
+        <f t="shared" si="11"/>
         <v>Doenca varchar(04) NOT NULL ,</v>
       </c>
       <c r="G43" s="9" t="str">
-        <f>MID(C43,9,2)</f>
+        <f t="shared" si="12"/>
         <v>04</v>
       </c>
       <c r="H43" s="6" t="s">
         <v>43</v>
       </c>
       <c r="I43" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E43,",obj.get",H43,"());")</f>
+        <f t="shared" si="9"/>
         <v>st.setString(42,obj.getDoenca());</v>
       </c>
       <c r="J43" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H43,",",G43,");")</f>
+        <f t="shared" si="10"/>
         <v>Constraints.setTextFieldMaxLength(idDoenca,04);</v>
       </c>
       <c r="K43" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setDoenca(rs.getString("Doenca"));</v>
       </c>
       <c r="L43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idDoenca.setText(aluno.getDoenca());</v>
       </c>
     </row>
@@ -2713,30 +2747,30 @@
         <v>43</v>
       </c>
       <c r="F44" s="2" t="str">
-        <f>_xlfn.CONCAT(B44," ",C44," ",D44," ,")</f>
+        <f t="shared" si="11"/>
         <v>DoencaQual varchar(60)   ,</v>
       </c>
       <c r="G44" s="9" t="str">
-        <f>MID(C44,9,2)</f>
+        <f t="shared" si="12"/>
         <v>60</v>
       </c>
       <c r="H44" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I44" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E44,",obj.get",H44,"());")</f>
+        <f t="shared" si="9"/>
         <v>st.setString(43,obj.getDoencaQual());</v>
       </c>
       <c r="J44" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H44,",",G44,");")</f>
+        <f t="shared" si="10"/>
         <v>Constraints.setTextFieldMaxLength(idDoencaQual,60);</v>
       </c>
       <c r="K44" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setDoencaQual(rs.getString("DoencaQual"));</v>
       </c>
       <c r="L44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idDoencaQual.setText(aluno.getDoencaQual());</v>
       </c>
     </row>
@@ -2757,30 +2791,30 @@
         <v>44</v>
       </c>
       <c r="F45" s="2" t="str">
-        <f>_xlfn.CONCAT(B45," ",C45," ",D45," ,")</f>
+        <f t="shared" si="11"/>
         <v>Remedio varchar(04) NOT NULL ,</v>
       </c>
       <c r="G45" s="9" t="str">
-        <f>MID(C45,9,2)</f>
+        <f t="shared" si="12"/>
         <v>04</v>
       </c>
       <c r="H45" s="6" t="s">
         <v>45</v>
       </c>
       <c r="I45" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E45,",obj.get",H45,"());")</f>
+        <f t="shared" si="9"/>
         <v>st.setString(44,obj.getRemedio());</v>
       </c>
       <c r="J45" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H45,",",G45,");")</f>
+        <f t="shared" si="10"/>
         <v>Constraints.setTextFieldMaxLength(idRemedio,04);</v>
       </c>
       <c r="K45" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setRemedio(rs.getString("Remedio"));</v>
       </c>
       <c r="L45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idRemedio.setText(aluno.getRemedio());</v>
       </c>
     </row>
@@ -2801,30 +2835,30 @@
         <v>45</v>
       </c>
       <c r="F46" s="2" t="str">
-        <f>_xlfn.CONCAT(B46," ",C46," ",D46," ,")</f>
+        <f t="shared" si="11"/>
         <v>RemedioQual varchar(60)   ,</v>
       </c>
       <c r="G46" s="9" t="str">
-        <f>MID(C46,9,2)</f>
+        <f t="shared" si="12"/>
         <v>60</v>
       </c>
       <c r="H46" s="6" t="s">
         <v>46</v>
       </c>
       <c r="I46" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E46,",obj.get",H46,"());")</f>
+        <f t="shared" si="9"/>
         <v>st.setString(45,obj.getRemedioQual());</v>
       </c>
       <c r="J46" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H46,",",G46,");")</f>
+        <f t="shared" si="10"/>
         <v>Constraints.setTextFieldMaxLength(idRemedioQual,60);</v>
       </c>
       <c r="K46" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setRemedioQual(rs.getString("RemedioQual"));</v>
       </c>
       <c r="L46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idRemedioQual.setText(aluno.getRemedioQual());</v>
       </c>
     </row>
@@ -2845,30 +2879,30 @@
         <v>46</v>
       </c>
       <c r="F47" s="2" t="str">
-        <f>_xlfn.CONCAT(B47," ",C47," ",D47," ,")</f>
+        <f t="shared" si="11"/>
         <v>BolsaFamilia varchar(04) NOT NULL ,</v>
       </c>
       <c r="G47" s="9" t="str">
-        <f>MID(C47,9,2)</f>
+        <f t="shared" si="12"/>
         <v>04</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>47</v>
       </c>
       <c r="I47" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E47,",obj.get",H47,"());")</f>
+        <f t="shared" si="9"/>
         <v>st.setString(46,obj.getBolsaFamilia());</v>
       </c>
       <c r="J47" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H47,",",G47,");")</f>
+        <f t="shared" si="10"/>
         <v>Constraints.setTextFieldMaxLength(idBolsaFamilia,04);</v>
       </c>
       <c r="K47" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setBolsaFamilia(rs.getString("BolsaFamilia"));</v>
       </c>
       <c r="L47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idBolsaFamilia.setText(aluno.getBolsaFamilia());</v>
       </c>
     </row>
@@ -2889,30 +2923,30 @@
         <v>47</v>
       </c>
       <c r="F48" s="2" t="str">
-        <f>_xlfn.CONCAT(B48," ",C48," ",D48," ,")</f>
+        <f t="shared" si="11"/>
         <v>Beneficio varchar(04) NOT NULL ,</v>
       </c>
       <c r="G48" s="9" t="str">
-        <f>MID(C48,9,2)</f>
+        <f t="shared" si="12"/>
         <v>04</v>
       </c>
       <c r="H48" s="6" t="s">
         <v>48</v>
       </c>
       <c r="I48" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E48,",obj.get",H48,"());")</f>
+        <f t="shared" si="9"/>
         <v>st.setString(47,obj.getBeneficio());</v>
       </c>
       <c r="J48" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H48,",",G48,");")</f>
+        <f t="shared" si="10"/>
         <v>Constraints.setTextFieldMaxLength(idBeneficio,04);</v>
       </c>
       <c r="K48" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setBeneficio(rs.getString("Beneficio"));</v>
       </c>
       <c r="L48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idBeneficio.setText(aluno.getBeneficio());</v>
       </c>
     </row>
@@ -2933,30 +2967,30 @@
         <v>48</v>
       </c>
       <c r="F49" s="2" t="str">
-        <f>_xlfn.CONCAT(B49," ",C49," ",D49," ,")</f>
+        <f t="shared" si="11"/>
         <v>CadastroUnico varchar(04) NOT NULL ,</v>
       </c>
       <c r="G49" s="9" t="str">
-        <f>MID(C49,9,2)</f>
+        <f t="shared" si="12"/>
         <v>04</v>
       </c>
       <c r="H49" s="6" t="s">
         <v>49</v>
       </c>
       <c r="I49" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E49,",obj.get",H49,"());")</f>
+        <f t="shared" si="9"/>
         <v>st.setString(48,obj.getCadastroUnico());</v>
       </c>
       <c r="J49" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H49,",",G49,");")</f>
+        <f t="shared" si="10"/>
         <v>Constraints.setTextFieldMaxLength(idCadastroUnico,04);</v>
       </c>
       <c r="K49" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setCadastroUnico(rs.getString("CadastroUnico"));</v>
       </c>
       <c r="L49" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idCadastroUnico.setText(aluno.getCadastroUnico());</v>
       </c>
     </row>
@@ -2977,7 +3011,7 @@
         <v>49</v>
       </c>
       <c r="F50" s="2" t="str">
-        <f>_xlfn.CONCAT(B50," ",C50," ",D50," ,")</f>
+        <f t="shared" si="11"/>
         <v>NumeroNIS int(11)   ,</v>
       </c>
       <c r="G50" s="9">
@@ -2987,19 +3021,19 @@
         <v>70</v>
       </c>
       <c r="I50" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E50,",obj.get",H50,"());")</f>
+        <f t="shared" si="9"/>
         <v>st.setString(49,obj.getNumeroNIS());</v>
       </c>
       <c r="J50" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H50,",",G50,");")</f>
+        <f t="shared" si="10"/>
         <v>Constraints.setTextFieldMaxLength(idNumeroNIS,11);</v>
       </c>
       <c r="K50" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setNumeroNIS(rs.getString("NumeroNIS"));</v>
       </c>
       <c r="L50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idNumeroNIS.setText(aluno.getNumeroNIS());</v>
       </c>
     </row>
@@ -3020,7 +3054,7 @@
         <v>50</v>
       </c>
       <c r="F51" s="2" t="str">
-        <f>_xlfn.CONCAT(B51," ",C51," ",D51," ,")</f>
+        <f t="shared" si="11"/>
         <v>Encaminha varchar(20) NOT NULL ,</v>
       </c>
       <c r="G51" s="9" t="str">
@@ -3031,19 +3065,19 @@
         <v>50</v>
       </c>
       <c r="I51" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E51,",obj.get",H51,"());")</f>
+        <f t="shared" si="9"/>
         <v>st.setString(50,obj.getEncaminha());</v>
       </c>
       <c r="J51" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H51,",",G51,");")</f>
+        <f t="shared" si="10"/>
         <v>Constraints.setTextFieldMaxLength(idEncaminha,20);</v>
       </c>
       <c r="K51" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setEncaminha(rs.getString("Encaminha"));</v>
       </c>
       <c r="L51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idEncaminha.setText(aluno.getEncaminha());</v>
       </c>
     </row>
@@ -3061,7 +3095,7 @@
         <v>51</v>
       </c>
       <c r="F52" s="2" t="str">
-        <f>_xlfn.CONCAT(B52," ",C52," ",D52," ,")</f>
+        <f t="shared" si="11"/>
         <v>EncaminhaOutra varchar(60)  ,</v>
       </c>
       <c r="G52" s="9" t="str">
@@ -3072,19 +3106,19 @@
         <v>51</v>
       </c>
       <c r="I52" t="str">
-        <f>_xlfn.CONCAT("st.setString(",E52,",obj.get",H52,"());")</f>
+        <f t="shared" si="9"/>
         <v>st.setString(51,obj.getEncaminhaOutra());</v>
       </c>
       <c r="J52" t="str">
-        <f>_xlfn.CONCAT("Constraints.setTextFieldMaxLength(id",H52,",",G52,");")</f>
+        <f t="shared" si="10"/>
         <v>Constraints.setTextFieldMaxLength(idEncaminhaOutra,60);</v>
       </c>
       <c r="K52" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>obj.setEncaminhaOutra(rs.getString("EncaminhaOutra"));</v>
       </c>
       <c r="L52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>idEncaminhaOutra.setText(aluno.getEncaminhaOutra());</v>
       </c>
     </row>
@@ -3359,10 +3393,883 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3308E0D-E73E-4DBE-AE01-D5628ADACB82}">
+  <dimension ref="A1:D60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="str">
+        <f>A1</f>
+        <v>CREATE TABLE aluno</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="str">
+        <f>A2</f>
+        <v>(id int  NOT NULL  AUTO_INCREMENT ,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="str">
+        <f>_xlfn.CONCAT(A3,"   ",B3,"  ",C3," ,")</f>
+        <v>NomeAluno   varchar(60)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" ref="D4:D57" si="0">_xlfn.CONCAT(A4,"   ",B4,"  ",C4," ,")</f>
+        <v>DataCadastro   DATE  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>Situacao   varchar(10)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>RgAluno   varchar(15)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>CpfAluno   varchar(15)    ,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>DataNascimentoAluno   DATE  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>Sexo   varchar(13)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>NomeRuaAluno   varchar(100)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>NumeroRuaAluno   int  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>BairroAluno   varchar(60)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>CepAluno   varchar(20)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>CelularAluno   varchar(15)    ,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>TelFixoAluno   varchar(20)    ,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>EmailAluno   varchar(60)    ,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>EscolaAluno   varchar(60)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>PeriodoAluno   varchar(10)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>AnoEscolarAluno   varchar(10)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>NomeMae   varchar(60)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>RgMae   varchar(15)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>CpfMae   varchar(15)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>CelularMae   varchar(15)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>NomePai   varchar(60)    ,</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>RgPai   varchar(15)    ,</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>CpfPai   varchar(15)    ,</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>CelularPai   varchar(15)    ,</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>NomeResponsavel   varchar(60)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>RgResponsavel   varchar(20)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>CpfResponsavel   varchar(15)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>CelularResponsavel   varchar(15)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>EnderecoTrabalho   varchar(60)    ,</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>NumeroTrabalho   int(04)    ,</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>CepTrabalho   varchar(20)    ,</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>Moradia   varchar(12)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>NumeroPessoasNaMoradia   int  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>Alergia   varchar(04)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>AlergiaQual   varchar(60)    ,</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>Deficiencia   varchar(04)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>DeficienciaQual   varchar(60)    ,</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>Cirurgia   varchar(04)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>CirurgiaQual   varchar(60)    ,</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>Doenca   varchar(04)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>DoencaQual   varchar(60)    ,</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>Remedio   varchar(04)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>RemedioQual   varchar(60)    ,</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" t="s">
+        <v>53</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>BolsaFamilia   varchar(04)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" t="s">
+        <v>53</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>Beneficio   varchar(04)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
+        <v>74</v>
+      </c>
+      <c r="C49" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>CadastroUnico   varchar(04)    ,</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" t="s">
+        <v>65</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>NumeroNIS   int    ,</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51" t="s">
+        <v>53</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>Encaminha   varchar(20)  NOT NULL ,</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>52</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>EncaminhaOutra   varchar(60)   ,</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>DataMatricula   DATE   ,</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v>DataExclusao   DATE   ,</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B55" t="s">
+        <v>64</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>TurmaRegular   varchar(20)   ,</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" t="s">
+        <v>64</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>TurmaEspecial   varchar(20)   ,</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>RendaFamiliar   int   ,</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>87</v>
+      </c>
+      <c r="D58" t="str">
+        <f>A58</f>
+        <v>UNIQUE KEY(CpfAluno) ,</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>69</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" ref="D59:D60" si="1">A59</f>
+        <v xml:space="preserve"> PRIMARY KEY (Id)</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>88</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="1"/>
+        <v>);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA6A3C9-69F0-4CB1-982B-4B74265FEC2E}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Report Relatorio PM finalizado
</commit_message>
<xml_diff>
--- a/Tabela_Aluno_Campos.xlsx
+++ b/Tabela_Aluno_Campos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jribe\eclipse-workspace\MariaLobatoGenteJovem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAB0E5F-A505-4726-BFC9-D741E94753AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE3E10D-2D89-4584-8B25-55BB3789EA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{BCEF3EA5-B1A7-48E7-889E-E8D820FE6D87}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="91">
   <si>
     <t>Integer</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>DATE</t>
+  </si>
+  <si>
+    <t>double</t>
   </si>
 </sst>
 </file>
@@ -2319,7 +2322,7 @@
         <v>34</v>
       </c>
       <c r="I34" t="str">
-        <f t="shared" ref="I34:I65" si="9">_xlfn.CONCAT("st.setString(",E34,",obj.get",H34,"());")</f>
+        <f t="shared" ref="I34:I52" si="9">_xlfn.CONCAT("st.setString(",E34,",obj.get",H34,"());")</f>
         <v>st.setString(33,obj.getCepTrabalho());</v>
       </c>
       <c r="J34" t="str">
@@ -3396,8 +3399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3308E0D-E73E-4DBE-AE01-D5628ADACB82}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D60" sqref="D1:D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4226,11 +4229,11 @@
         <v>84</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="D57" t="str">
         <f t="shared" si="0"/>
-        <v>RendaFamiliar   int   ,</v>
+        <v>RendaFamiliar   double   ,</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>